<commit_message>
update 29/12/2023 (Gần ok)
</commit_message>
<xml_diff>
--- a/TonKho.xlsx
+++ b/TonKho.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -98,7 +98,7 @@
     <t>5000</t>
   </si>
   <si>
-    <t>45</t>
+    <t>39</t>
   </si>
   <si>
     <t>xiaomi</t>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>ss</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -258,7 +255,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -298,7 +295,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>

</xml_diff>